<commit_message>
Simplifies main into two functions "Calibrate" and "Simulate". See script "run_tests" for an example on calling these functions
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JFV09\Dropbox\Git\india-subnational\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C1B45B-D14E-4871-B892-9F57B35B81A1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50D6DC7-F40D-4053-9E63-69549473AD32}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="5310" windowWidth="21600" windowHeight="12735" xr2:uid="{EFBC62C4-A86B-45CA-BA7A-8E0631C64F4B}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="12735" xr2:uid="{EFBC62C4-A86B-45CA-BA7A-8E0631C64F4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,7 +433,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Now modified to calibrate for all DTO districts
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JFV09\Dropbox\Git\india-subnational\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50D6DC7-F40D-4053-9E63-69549473AD32}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E54827-1309-403D-B9B7-E8AC062415C3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="12735" xr2:uid="{EFBC62C4-A86B-45CA-BA7A-8E0631C64F4B}"/>
+    <workbookView xWindow="0" yWindow="1305" windowWidth="19200" windowHeight="10095" xr2:uid="{EFBC62C4-A86B-45CA-BA7A-8E0631C64F4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,7 +433,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>